<commit_message>
Added SubClasses for Players
added subclasses and ComboBox Listeners for Subclasses
</commit_message>
<xml_diff>
--- a/DnD Suite/sample.xlsx
+++ b/DnD Suite/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Naser Salameh\OneDrive - University of Southampton\Coding Workspaces\Java\eclipse-workspace\DnD_Suite\DnD Suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9187CEC-C55C-4A2F-8200-DB74607658F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7309A246-E11F-4413-A5DC-35BC6CD561DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="334">
   <si>
     <t>Player</t>
   </si>
@@ -1186,12 +1186,6 @@
   </si>
   <si>
     <t>Speed</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Beast Master</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lore College</t>
   </si>
   <si>
     <t>Subclass</t>
@@ -1631,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1642,16 +1636,16 @@
     <col min="1" max="1" width="24.77734375" customWidth="1"/>
     <col min="2" max="2" width="15.77734375" customWidth="1"/>
     <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="3"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" customWidth="1"/>
-    <col min="16" max="16" width="15.77734375" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="3"/>
+    <col min="10" max="10" width="12.5546875" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>70</v>
       </c>
@@ -1662,52 +1656,52 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1718,49 +1712,49 @@
         <v>202</v>
       </c>
       <c r="D2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>200</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>10</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>12</v>
-      </c>
-      <c r="I2">
-        <v>13</v>
       </c>
       <c r="J2">
         <v>13</v>
       </c>
       <c r="K2">
+        <v>13</v>
+      </c>
+      <c r="L2">
         <v>15</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>16</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>20</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>30</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>4</v>
       </c>
-      <c r="P2" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1771,49 +1765,49 @@
         <v>201</v>
       </c>
       <c r="D3" t="s">
+        <v>287</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>130</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>10</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>12</v>
-      </c>
-      <c r="I3">
-        <v>13</v>
       </c>
       <c r="J3">
         <v>13</v>
       </c>
       <c r="K3">
+        <v>13</v>
+      </c>
+      <c r="L3">
         <v>15</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>16</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>23</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>25</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>2</v>
       </c>
-      <c r="P3" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1824,49 +1818,49 @@
         <v>195</v>
       </c>
       <c r="D4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>2</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>100</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>10</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>12</v>
-      </c>
-      <c r="I4">
-        <v>13</v>
       </c>
       <c r="J4">
         <v>13</v>
       </c>
       <c r="K4">
+        <v>13</v>
+      </c>
+      <c r="L4">
         <v>15</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>16</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>18</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>20</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>1</v>
       </c>
-      <c r="P4" t="s">
-        <v>334</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1877,52 +1871,52 @@
         <v>204</v>
       </c>
       <c r="D5" t="s">
+        <v>312</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>200</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>10</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>12</v>
-      </c>
-      <c r="I5">
-        <v>13</v>
       </c>
       <c r="J5">
         <v>13</v>
       </c>
       <c r="K5">
+        <v>13</v>
+      </c>
+      <c r="L5">
         <v>15</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>16</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>11</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>30</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>1</v>
       </c>
-      <c r="P5" t="s">
-        <v>312</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>27</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1933,45 +1927,45 @@
         <v>200</v>
       </c>
       <c r="D6" t="s">
+        <v>285</v>
+      </c>
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>150</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>10</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>12</v>
-      </c>
-      <c r="I6">
-        <v>13</v>
       </c>
       <c r="J6">
         <v>13</v>
       </c>
       <c r="K6">
+        <v>13</v>
+      </c>
+      <c r="L6">
         <v>15</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>16</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>10</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>30</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0</v>
       </c>
-      <c r="P6" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Npc GUI Fully Done
Fully remodeled NPC, added NPC GUI, Controller and Parser
</commit_message>
<xml_diff>
--- a/DnD Suite/sample.xlsx
+++ b/DnD Suite/sample.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Naser Salameh\OneDrive - University of Southampton\Coding Workspaces\Java\eclipse-workspace\DnD_Suite\DnD Suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7309A246-E11F-4413-A5DC-35BC6CD561DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A5BC5B-F1C7-4FC8-9941-BB74D2901DFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Players" sheetId="1" r:id="rId1"/>
+    <sheet name="Races" sheetId="10" r:id="rId1"/>
     <sheet name="Classes" sheetId="9" r:id="rId2"/>
-    <sheet name="Races" sheetId="10" r:id="rId3"/>
-    <sheet name="Time-Pieces" sheetId="2" r:id="rId4"/>
-    <sheet name="Time-Anomalies" sheetId="3" r:id="rId5"/>
-    <sheet name="Quests" sheetId="4" r:id="rId6"/>
-    <sheet name="Items" sheetId="5" r:id="rId7"/>
-    <sheet name="NPCs" sheetId="6" r:id="rId8"/>
+    <sheet name="Players" sheetId="1" r:id="rId3"/>
+    <sheet name="NPCs" sheetId="6" r:id="rId4"/>
+    <sheet name="Time-Pieces" sheetId="2" r:id="rId5"/>
+    <sheet name="Time-Anomalies" sheetId="3" r:id="rId6"/>
+    <sheet name="Quests" sheetId="4" r:id="rId7"/>
+    <sheet name="Items" sheetId="5" r:id="rId8"/>
     <sheet name="Thedas" sheetId="7" r:id="rId9"/>
     <sheet name="Snitel" sheetId="8" r:id="rId10"/>
   </sheets>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="333">
   <si>
     <t>Player</t>
   </si>
@@ -359,9 +359,6 @@
     <t>Session</t>
   </si>
   <si>
-    <t>Description, Age</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
@@ -369,9 +366,6 @@
   </si>
   <si>
     <t>Prologue</t>
-  </si>
-  <si>
-    <t>Disheveled Wizard, 18</t>
   </si>
   <si>
     <r>
@@ -405,9 +399,6 @@
     <t>Azor</t>
   </si>
   <si>
-    <t>Assassin, 34</t>
-  </si>
-  <si>
     <t>Pre-New Era: Orlesian assassin, was hired to kill the party.
 New Era: Assassin for hire, easter egg appearances</t>
   </si>
@@ -416,9 +407,6 @@
   </si>
   <si>
     <t>Duke Lapas</t>
-  </si>
-  <si>
-    <t>Duke, 56</t>
   </si>
   <si>
     <t>Murdered nameless's parents and took ownership of the region.
@@ -428,13 +416,7 @@
 Theodore and Colletta, by threating Colletta's parents</t>
   </si>
   <si>
-    <t>Orlais, Val Pris</t>
-  </si>
-  <si>
     <t>Lord Timber</t>
-  </si>
-  <si>
-    <t>Lord, 45</t>
   </si>
   <si>
     <t>Lord of Lothering, stupid but honorable, fat, pretends to be smart.
@@ -447,25 +429,16 @@
     <t>Marcus</t>
   </si>
   <si>
-    <t>Lord's son, 8</t>
-  </si>
-  <si>
     <t>Kidnapped son of Lord Timber, fat bully</t>
   </si>
   <si>
     <t>Smithy samson</t>
   </si>
   <si>
-    <t>Lothering local blacksmith , 50</t>
-  </si>
-  <si>
     <t>Normal Smith</t>
   </si>
   <si>
     <t>Samson Junior</t>
-  </si>
-  <si>
-    <t>Smithy's son. 18</t>
   </si>
   <si>
     <t>dreams of leaving lothering and learning how to forge heroic weapons</t>
@@ -1189,6 +1162,30 @@
   </si>
   <si>
     <t>Subclass</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Smithy's son</t>
+  </si>
+  <si>
+    <t>Lothering local blacksmith</t>
+  </si>
+  <si>
+    <t>Lord's son</t>
+  </si>
+  <si>
+    <t>Lord</t>
+  </si>
+  <si>
+    <t>Duke</t>
+  </si>
+  <si>
+    <t>Disheveled Wizard</t>
+  </si>
+  <si>
+    <t>Thedas</t>
   </si>
 </sst>
 </file>
@@ -1624,10 +1621,737 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6823123-7AB7-435E-B2CB-BAEFFD54B1B2}">
+  <dimension ref="A1:A30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
+        <v>6</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15">
+        <v>9</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>100</v>
+      </c>
+      <c r="B15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE1A93B-D08A-48A9-8BEF-92544091AFA6}">
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G4" t="s">
+        <v>239</v>
+      </c>
+      <c r="H4" t="s">
+        <v>240</v>
+      </c>
+      <c r="I4" t="s">
+        <v>241</v>
+      </c>
+      <c r="J4" t="s">
+        <v>242</v>
+      </c>
+      <c r="K4" t="s">
+        <v>243</v>
+      </c>
+      <c r="L4" t="s">
+        <v>245</v>
+      </c>
+      <c r="M4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6" t="s">
+        <v>253</v>
+      </c>
+      <c r="D6" t="s">
+        <v>254</v>
+      </c>
+      <c r="E6" t="s">
+        <v>255</v>
+      </c>
+      <c r="F6" t="s">
+        <v>256</v>
+      </c>
+      <c r="G6" t="s">
+        <v>257</v>
+      </c>
+      <c r="H6" t="s">
+        <v>258</v>
+      </c>
+      <c r="I6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J6" t="s">
+        <v>260</v>
+      </c>
+      <c r="K6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D7" t="s">
+        <v>264</v>
+      </c>
+      <c r="E7" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" t="s">
+        <v>266</v>
+      </c>
+      <c r="G7" t="s">
+        <v>267</v>
+      </c>
+      <c r="H7" t="s">
+        <v>268</v>
+      </c>
+      <c r="I7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C8" t="s">
+        <v>271</v>
+      </c>
+      <c r="D8" t="s">
+        <v>272</v>
+      </c>
+      <c r="E8" t="s">
+        <v>273</v>
+      </c>
+      <c r="F8" t="s">
+        <v>274</v>
+      </c>
+      <c r="G8" t="s">
+        <v>275</v>
+      </c>
+      <c r="H8" t="s">
+        <v>276</v>
+      </c>
+      <c r="I8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C9" t="s">
+        <v>279</v>
+      </c>
+      <c r="D9" t="s">
+        <v>280</v>
+      </c>
+      <c r="E9" t="s">
+        <v>281</v>
+      </c>
+      <c r="F9" t="s">
+        <v>282</v>
+      </c>
+      <c r="G9" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" t="s">
+        <v>284</v>
+      </c>
+      <c r="C10" t="s">
+        <v>285</v>
+      </c>
+      <c r="D10" t="s">
+        <v>286</v>
+      </c>
+      <c r="E10" t="s">
+        <v>287</v>
+      </c>
+      <c r="F10" t="s">
+        <v>288</v>
+      </c>
+      <c r="G10" t="s">
+        <v>289</v>
+      </c>
+      <c r="H10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B11" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" t="s">
+        <v>292</v>
+      </c>
+      <c r="D11" t="s">
+        <v>293</v>
+      </c>
+      <c r="E11" t="s">
+        <v>294</v>
+      </c>
+      <c r="F11" t="s">
+        <v>295</v>
+      </c>
+      <c r="G11" t="s">
+        <v>296</v>
+      </c>
+      <c r="H11" t="s">
+        <v>297</v>
+      </c>
+      <c r="I11" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" t="s">
+        <v>299</v>
+      </c>
+      <c r="C12" t="s">
+        <v>300</v>
+      </c>
+      <c r="D12" t="s">
+        <v>301</v>
+      </c>
+      <c r="E12" t="s">
+        <v>302</v>
+      </c>
+      <c r="F12" t="s">
+        <v>303</v>
+      </c>
+      <c r="G12" t="s">
+        <v>304</v>
+      </c>
+      <c r="H12" t="s">
+        <v>305</v>
+      </c>
+      <c r="I12" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" t="s">
+        <v>307</v>
+      </c>
+      <c r="C13" t="s">
+        <v>308</v>
+      </c>
+      <c r="D13" t="s">
+        <v>309</v>
+      </c>
+      <c r="E13" t="s">
+        <v>310</v>
+      </c>
+      <c r="F13" t="s">
+        <v>311</v>
+      </c>
+      <c r="G13" t="s">
+        <v>312</v>
+      </c>
+      <c r="H13" t="s">
+        <v>313</v>
+      </c>
+      <c r="I13" t="s">
+        <v>314</v>
+      </c>
+      <c r="J13" t="s">
+        <v>315</v>
+      </c>
+      <c r="K13" t="s">
+        <v>316</v>
+      </c>
+      <c r="L13" t="s">
+        <v>317</v>
+      </c>
+      <c r="M13" t="s">
+        <v>318</v>
+      </c>
+      <c r="N13" t="s">
+        <v>319</v>
+      </c>
+      <c r="O13" t="s">
+        <v>320</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1656,7 +2380,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1665,7 +2389,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -1686,10 +2410,10 @@
         <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>4</v>
@@ -1709,10 +2433,10 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D2" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -1762,10 +2486,10 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -1815,10 +2539,10 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D4" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -1865,13 +2589,13 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D5" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1924,10 +2648,10 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D6" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
@@ -1975,174 +2699,205 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C15"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="1" max="2" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
-        <v>2</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="B5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
-        <v>5</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15">
-        <v>6</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12">
-        <v>7</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15">
-        <v>9</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B12" t="s">
-        <v>185</v>
-      </c>
-      <c r="C12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
-        <v>11</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B14" t="s">
-        <v>189</v>
-      </c>
-      <c r="C14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>100</v>
-      </c>
-      <c r="B15" t="s">
-        <v>191</v>
+      <c r="C1" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2">
+        <v>18</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>329</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>327</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2150,559 +2905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE1A93B-D08A-48A9-8BEF-92544091AFA6}">
-  <dimension ref="A1:O13"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D2" t="s">
-        <v>233</v>
-      </c>
-      <c r="E2" t="s">
-        <v>234</v>
-      </c>
-      <c r="F2" t="s">
-        <v>235</v>
-      </c>
-      <c r="G2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C3" t="s">
-        <v>238</v>
-      </c>
-      <c r="D3" t="s">
-        <v>239</v>
-      </c>
-      <c r="E3" t="s">
-        <v>240</v>
-      </c>
-      <c r="F3" t="s">
-        <v>241</v>
-      </c>
-      <c r="G3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>196</v>
-      </c>
-      <c r="B4" t="s">
-        <v>243</v>
-      </c>
-      <c r="C4" t="s">
-        <v>244</v>
-      </c>
-      <c r="D4" t="s">
-        <v>245</v>
-      </c>
-      <c r="E4" t="s">
-        <v>246</v>
-      </c>
-      <c r="F4" t="s">
-        <v>247</v>
-      </c>
-      <c r="G4" t="s">
-        <v>248</v>
-      </c>
-      <c r="H4" t="s">
-        <v>249</v>
-      </c>
-      <c r="I4" t="s">
-        <v>250</v>
-      </c>
-      <c r="J4" t="s">
-        <v>251</v>
-      </c>
-      <c r="K4" t="s">
-        <v>252</v>
-      </c>
-      <c r="L4" t="s">
-        <v>254</v>
-      </c>
-      <c r="M4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>197</v>
-      </c>
-      <c r="B5" t="s">
-        <v>255</v>
-      </c>
-      <c r="C5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D5" t="s">
-        <v>257</v>
-      </c>
-      <c r="E5" t="s">
-        <v>258</v>
-      </c>
-      <c r="F5" t="s">
-        <v>259</v>
-      </c>
-      <c r="G5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>198</v>
-      </c>
-      <c r="B6" t="s">
-        <v>261</v>
-      </c>
-      <c r="C6" t="s">
-        <v>262</v>
-      </c>
-      <c r="D6" t="s">
-        <v>263</v>
-      </c>
-      <c r="E6" t="s">
-        <v>264</v>
-      </c>
-      <c r="F6" t="s">
-        <v>265</v>
-      </c>
-      <c r="G6" t="s">
-        <v>266</v>
-      </c>
-      <c r="H6" t="s">
-        <v>267</v>
-      </c>
-      <c r="I6" t="s">
-        <v>268</v>
-      </c>
-      <c r="J6" t="s">
-        <v>269</v>
-      </c>
-      <c r="K6" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>199</v>
-      </c>
-      <c r="B7" t="s">
-        <v>271</v>
-      </c>
-      <c r="C7" t="s">
-        <v>272</v>
-      </c>
-      <c r="D7" t="s">
-        <v>273</v>
-      </c>
-      <c r="E7" t="s">
-        <v>274</v>
-      </c>
-      <c r="F7" t="s">
-        <v>275</v>
-      </c>
-      <c r="G7" t="s">
-        <v>276</v>
-      </c>
-      <c r="H7" t="s">
-        <v>277</v>
-      </c>
-      <c r="I7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>200</v>
-      </c>
-      <c r="B8" t="s">
-        <v>279</v>
-      </c>
-      <c r="C8" t="s">
-        <v>280</v>
-      </c>
-      <c r="D8" t="s">
-        <v>281</v>
-      </c>
-      <c r="E8" t="s">
-        <v>282</v>
-      </c>
-      <c r="F8" t="s">
-        <v>283</v>
-      </c>
-      <c r="G8" t="s">
-        <v>284</v>
-      </c>
-      <c r="H8" t="s">
-        <v>285</v>
-      </c>
-      <c r="I8" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>201</v>
-      </c>
-      <c r="B9" t="s">
-        <v>287</v>
-      </c>
-      <c r="C9" t="s">
-        <v>288</v>
-      </c>
-      <c r="D9" t="s">
-        <v>289</v>
-      </c>
-      <c r="E9" t="s">
-        <v>290</v>
-      </c>
-      <c r="F9" t="s">
-        <v>291</v>
-      </c>
-      <c r="G9" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>202</v>
-      </c>
-      <c r="B10" t="s">
-        <v>293</v>
-      </c>
-      <c r="C10" t="s">
-        <v>294</v>
-      </c>
-      <c r="D10" t="s">
-        <v>295</v>
-      </c>
-      <c r="E10" t="s">
-        <v>296</v>
-      </c>
-      <c r="F10" t="s">
-        <v>297</v>
-      </c>
-      <c r="G10" t="s">
-        <v>298</v>
-      </c>
-      <c r="H10" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B11" t="s">
-        <v>300</v>
-      </c>
-      <c r="C11" t="s">
-        <v>301</v>
-      </c>
-      <c r="D11" t="s">
-        <v>302</v>
-      </c>
-      <c r="E11" t="s">
-        <v>303</v>
-      </c>
-      <c r="F11" t="s">
-        <v>304</v>
-      </c>
-      <c r="G11" t="s">
-        <v>305</v>
-      </c>
-      <c r="H11" t="s">
-        <v>306</v>
-      </c>
-      <c r="I11" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>204</v>
-      </c>
-      <c r="B12" t="s">
-        <v>308</v>
-      </c>
-      <c r="C12" t="s">
-        <v>309</v>
-      </c>
-      <c r="D12" t="s">
-        <v>310</v>
-      </c>
-      <c r="E12" t="s">
-        <v>311</v>
-      </c>
-      <c r="F12" t="s">
-        <v>312</v>
-      </c>
-      <c r="G12" t="s">
-        <v>313</v>
-      </c>
-      <c r="H12" t="s">
-        <v>314</v>
-      </c>
-      <c r="I12" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>205</v>
-      </c>
-      <c r="B13" t="s">
-        <v>316</v>
-      </c>
-      <c r="C13" t="s">
-        <v>317</v>
-      </c>
-      <c r="D13" t="s">
-        <v>318</v>
-      </c>
-      <c r="E13" t="s">
-        <v>319</v>
-      </c>
-      <c r="F13" t="s">
-        <v>320</v>
-      </c>
-      <c r="G13" t="s">
-        <v>321</v>
-      </c>
-      <c r="H13" t="s">
-        <v>322</v>
-      </c>
-      <c r="I13" t="s">
-        <v>323</v>
-      </c>
-      <c r="J13" t="s">
-        <v>324</v>
-      </c>
-      <c r="K13" t="s">
-        <v>325</v>
-      </c>
-      <c r="L13" t="s">
-        <v>326</v>
-      </c>
-      <c r="M13" t="s">
-        <v>327</v>
-      </c>
-      <c r="N13" t="s">
-        <v>328</v>
-      </c>
-      <c r="O13" t="s">
-        <v>329</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6823123-7AB7-435E-B2CB-BAEFFD54B1B2}">
-  <dimension ref="A1:A30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -2776,7 +2979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -2857,7 +3060,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -2965,7 +3168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2995,145 +3198,6 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" t="s">
-        <v>89</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
@@ -3157,206 +3221,206 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ImageParser and PlayerParser
Set up an image parser for portraits and implemented PlayerPortrait Parser
</commit_message>
<xml_diff>
--- a/DnD Suite/sample.xlsx
+++ b/DnD Suite/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Naser Salameh\OneDrive - University of Southampton\Coding Workspaces\Java\eclipse-workspace\DnD_Suite\DnD Suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A5BC5B-F1C7-4FC8-9941-BB74D2901DFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637BAF72-0A29-469A-80F9-D21B4108A318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Races" sheetId="10" r:id="rId1"/>
@@ -2351,8 +2351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2703,8 +2703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3064,7 +3064,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Location Model, GUI, Controller and Parser
Added Location, fully functional (needs better JTree nesting)
</commit_message>
<xml_diff>
--- a/DnD Suite/sample.xlsx
+++ b/DnD Suite/sample.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Naser Salameh\OneDrive - University of Southampton\Coding Workspaces\Java\eclipse-workspace\DnD_Suite\DnD Suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637BAF72-0A29-469A-80F9-D21B4108A318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0B6BD1-CD29-409B-915A-0928DFCA6391}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Races" sheetId="10" r:id="rId1"/>
     <sheet name="Classes" sheetId="9" r:id="rId2"/>
     <sheet name="Players" sheetId="1" r:id="rId3"/>
     <sheet name="NPCs" sheetId="6" r:id="rId4"/>
-    <sheet name="Time-Pieces" sheetId="2" r:id="rId5"/>
-    <sheet name="Time-Anomalies" sheetId="3" r:id="rId6"/>
-    <sheet name="Quests" sheetId="4" r:id="rId7"/>
-    <sheet name="Items" sheetId="5" r:id="rId8"/>
-    <sheet name="Thedas" sheetId="7" r:id="rId9"/>
+    <sheet name="Locations" sheetId="7" r:id="rId5"/>
+    <sheet name="Time-Pieces" sheetId="2" r:id="rId6"/>
+    <sheet name="Time-Anomalies" sheetId="3" r:id="rId7"/>
+    <sheet name="Quests" sheetId="4" r:id="rId8"/>
+    <sheet name="Items" sheetId="5" r:id="rId9"/>
     <sheet name="Snitel" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="337">
   <si>
     <t>Player</t>
   </si>
@@ -1186,6 +1186,18 @@
   </si>
   <si>
     <t>Thedas</t>
+  </si>
+  <si>
+    <t>World</t>
+  </si>
+  <si>
+    <t>Various</t>
+  </si>
+  <si>
+    <t>Within</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1262,7 +1274,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1307,6 +1319,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2351,7 +2364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2906,6 +2919,290 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.88671875" customWidth="1"/>
+    <col min="6" max="6" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>332</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>332</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" t="s">
+        <v>332</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" t="s">
+        <v>332</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" t="s">
+        <v>332</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>332</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
+        <v>332</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" t="s">
+        <v>332</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" t="s">
+        <v>332</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -2979,7 +3276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -3060,7 +3357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -3170,7 +3467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3203,230 +3500,4 @@
   </sheetData>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.88671875" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
-  <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Items and NPC GUI
Fixed bugs
</commit_message>
<xml_diff>
--- a/DnD Suite/sample.xlsx
+++ b/DnD Suite/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Naser Salameh\OneDrive - University of Southampton\Coding Workspaces\Java\eclipse-workspace\DnD_Suite\DnD Suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0B6BD1-CD29-409B-915A-0928DFCA6391}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDDBC40-BF22-4688-8639-92890E9B9F9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Races" sheetId="10" r:id="rId1"/>
@@ -18,18 +18,25 @@
     <sheet name="Players" sheetId="1" r:id="rId3"/>
     <sheet name="NPCs" sheetId="6" r:id="rId4"/>
     <sheet name="Locations" sheetId="7" r:id="rId5"/>
-    <sheet name="Time-Pieces" sheetId="2" r:id="rId6"/>
-    <sheet name="Time-Anomalies" sheetId="3" r:id="rId7"/>
-    <sheet name="Quests" sheetId="4" r:id="rId8"/>
-    <sheet name="Items" sheetId="5" r:id="rId9"/>
+    <sheet name="Items" sheetId="5" r:id="rId6"/>
+    <sheet name="Time-Pieces" sheetId="2" r:id="rId7"/>
+    <sheet name="Time-Anomalies" sheetId="3" r:id="rId8"/>
+    <sheet name="Quests" sheetId="4" r:id="rId9"/>
     <sheet name="Snitel" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="342">
   <si>
     <t>Player</t>
   </si>
@@ -347,9 +354,6 @@
     <t>Heart of a Blade</t>
   </si>
   <si>
-    <t>Item Name</t>
-  </si>
-  <si>
     <t>Owned By</t>
   </si>
   <si>
@@ -1198,6 +1202,24 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Rarity</t>
+  </si>
+  <si>
+    <t>Attributes</t>
+  </si>
+  <si>
+    <t>Sword</t>
+  </si>
+  <si>
+    <t>A sword</t>
+  </si>
+  <si>
+    <t>+2 attack</t>
+  </si>
+  <si>
+    <t>Common</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1320,6 +1342,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1653,7 +1676,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -1673,32 +1696,32 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
@@ -1708,92 +1731,92 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -1818,13 +1841,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" t="s">
         <v>149</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>150</v>
-      </c>
-      <c r="C1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1832,18 +1855,18 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" t="s">
         <v>153</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>154</v>
-      </c>
-      <c r="C3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -1851,32 +1874,32 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>156</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" t="s">
         <v>158</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>159</v>
-      </c>
-      <c r="C5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" t="s">
         <v>161</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>162</v>
-      </c>
-      <c r="C6" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -1884,10 +1907,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>164</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -1895,10 +1918,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>166</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -1906,21 +1929,21 @@
         <v>7</v>
       </c>
       <c r="B9" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>168</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" t="s">
         <v>170</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>171</v>
-      </c>
-      <c r="C10" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -1928,21 +1951,21 @@
         <v>9</v>
       </c>
       <c r="B11" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>173</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" t="s">
         <v>175</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>176</v>
-      </c>
-      <c r="C12" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -1950,18 +1973,18 @@
         <v>11</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" t="s">
         <v>179</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>180</v>
-      </c>
-      <c r="C14" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1969,7 +1992,7 @@
         <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1992,367 +2015,367 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" t="s">
         <v>222</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>223</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>224</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>225</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>226</v>
-      </c>
-      <c r="G2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" t="s">
         <v>228</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>229</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>230</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>231</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>232</v>
-      </c>
-      <c r="G3" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" t="s">
         <v>234</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>235</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>236</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>237</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>238</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>239</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>240</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>241</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>242</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
+        <v>244</v>
+      </c>
+      <c r="M4" t="s">
         <v>243</v>
-      </c>
-      <c r="L4" t="s">
-        <v>245</v>
-      </c>
-      <c r="M4" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C5" t="s">
         <v>246</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>247</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>248</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>249</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>250</v>
-      </c>
-      <c r="G5" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" t="s">
         <v>252</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>253</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>254</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>255</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>256</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>257</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>258</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>259</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>260</v>
-      </c>
-      <c r="K6" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B7" t="s">
+        <v>261</v>
+      </c>
+      <c r="C7" t="s">
         <v>262</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>263</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>264</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>265</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>266</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>267</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>268</v>
-      </c>
-      <c r="I7" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" t="s">
         <v>270</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>271</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>272</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>273</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>274</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>275</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>276</v>
-      </c>
-      <c r="I8" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" t="s">
         <v>278</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>279</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>280</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>281</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>282</v>
-      </c>
-      <c r="G9" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C10" t="s">
         <v>284</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>285</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>286</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>287</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>288</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>289</v>
-      </c>
-      <c r="H10" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B11" t="s">
+        <v>290</v>
+      </c>
+      <c r="C11" t="s">
         <v>291</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>292</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>293</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>294</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>295</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>296</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>297</v>
-      </c>
-      <c r="I11" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B12" t="s">
+        <v>298</v>
+      </c>
+      <c r="C12" t="s">
         <v>299</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>300</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>301</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>302</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>303</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>304</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>305</v>
-      </c>
-      <c r="I12" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B13" t="s">
+        <v>306</v>
+      </c>
+      <c r="C13" t="s">
         <v>307</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>308</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>309</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>310</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>311</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>312</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>313</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>314</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>315</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>316</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>317</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>318</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>319</v>
-      </c>
-      <c r="O13" t="s">
-        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -2384,7 +2407,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2393,7 +2416,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -2402,7 +2425,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -2423,10 +2446,10 @@
         <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>323</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>4</v>
@@ -2446,10 +2469,10 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -2499,10 +2522,10 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -2552,10 +2575,10 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -2602,13 +2625,13 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -2661,10 +2684,10 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
@@ -2731,22 +2754,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>54</v>
@@ -2754,163 +2777,163 @@
     </row>
     <row r="2" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C2">
         <v>18</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>331</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3">
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
         <v>77</v>
-      </c>
-      <c r="G3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4">
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C5">
         <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" t="s">
         <v>82</v>
-      </c>
-      <c r="G5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6">
         <v>8</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7">
         <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C8">
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2922,7 +2945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2938,39 +2961,39 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>336</v>
-      </c>
-      <c r="C2" s="18" t="s">
+      <c r="D2" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>334</v>
-      </c>
       <c r="E2" s="18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>46</v>
@@ -2978,222 +3001,222 @@
     </row>
     <row r="3" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B3" t="s">
-        <v>332</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="10" t="s">
         <v>98</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>331</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B5" t="s">
-        <v>332</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B6" t="s">
-        <v>332</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B7" t="s">
-        <v>332</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" t="s">
+        <v>331</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B8" t="s">
-        <v>332</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>331</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B9" t="s">
-        <v>332</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" t="s">
+        <v>331</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B10" t="s">
-        <v>332</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" t="s">
+        <v>331</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B11" t="s">
-        <v>332</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" t="s">
+        <v>331</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B12" t="s">
-        <v>332</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="6" t="s">
         <v>142</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" t="s">
+        <v>331</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B13" t="s">
-        <v>332</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3203,6 +3226,64 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="56.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="D2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -3276,7 +3357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -3357,7 +3438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -3465,39 +3546,4 @@
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.21875" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
-</worksheet>
 </file>
</xml_diff>